<commit_message>
Dec 31 last updated
</commit_message>
<xml_diff>
--- a/input/investment & growth.xlsx
+++ b/input/investment & growth.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Course &amp; Studies\Software\work area\Repos\Investment Analysis - A Statistical Perspective\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFFE1870-8ED9-434A-A037-F6995A72BF14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC0F9131-E8CD-40BD-9817-FD0F4E79295D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" activeTab="3" xr2:uid="{C4A2AE80-0629-47E2-9608-DEE60C8860FC}"/>
   </bookViews>
@@ -496,7 +496,7 @@
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1120,20 +1120,29 @@
       <c r="B29">
         <v>2025</v>
       </c>
+      <c r="C29">
+        <v>1103.5</v>
+      </c>
+      <c r="D29">
+        <v>6000</v>
+      </c>
+      <c r="E29">
+        <v>3000</v>
+      </c>
       <c r="H29">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="J29">
-        <v>270</v>
+        <v>310</v>
       </c>
       <c r="K29">
         <f t="shared" si="1"/>
-        <v>270</v>
+        <v>10413.5</v>
       </c>
       <c r="L29">
         <f>SUM($K$2:K29)</f>
-        <v>9842.52</v>
+        <v>19986.02</v>
       </c>
     </row>
   </sheetData>
@@ -1147,7 +1156,7 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1720,24 +1729,24 @@
         <v>2025</v>
       </c>
       <c r="C29">
-        <v>5216.07</v>
+        <v>6404.3</v>
       </c>
       <c r="D29">
-        <v>1353</v>
+        <v>7340</v>
       </c>
       <c r="E29">
-        <v>3016.82</v>
+        <v>6020</v>
       </c>
       <c r="H29">
         <f t="shared" si="0"/>
-        <v>3016.82</v>
+        <v>6020</v>
       </c>
       <c r="J29">
-        <v>718.02</v>
+        <v>737.63</v>
       </c>
       <c r="K29">
         <f t="shared" si="1"/>
-        <v>10303.91</v>
+        <v>20501.93</v>
       </c>
     </row>
   </sheetData>
@@ -1849,7 +1858,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>